<commit_message>
fix campi opzionali test case 24
</commit_message>
<xml_diff>
--- a/GATEWAY/SIG120200_00987654321-AppTest01/Replycare s.r.l./Med58/V.1.0.0/report-checklist.xlsx
+++ b/GATEWAY/SIG120200_00987654321-AppTest01/Replycare s.r.l./Med58/V.1.0.0/report-checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albertor\Desktop\FSE\accreditamento\V.1.0.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albertor\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1730,13 +1730,13 @@
     <t>Errore durante il caricamento del documento. C'è stato un errore durante la comunicazione con il Fascicolo Sanitario Elettronico, la preghiamo di [riprovare la procedura. Se l'errore persiste] comunicare con support@med58.com</t>
   </si>
   <si>
-    <t>2025-07-15T14:27:09Z</t>
-  </si>
-  <si>
-    <t>eef502286904a3b83eac486c3d2938b4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.122c21eed48ab00881085e203a13c8e9439a0d1ae9f767908715d2ed0c67b945.a84e29462c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-09-23T07:29:59Z</t>
+  </si>
+  <si>
+    <t>f52034d7da53734ac1d19c924c54c106</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.ba80ab8fc9448e3415859a7372caee1392cfdf2fdbbb7a6041718f1e61d2f3cb.4c7000a530^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3806,10 +3806,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I192" sqref="I192:I193"/>
+      <selection pane="bottomRight" activeCell="A166" sqref="A166:XFD166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9985,7 +9985,7 @@
         <v>389</v>
       </c>
       <c r="F166" s="37">
-        <v>45853</v>
+        <v>45923</v>
       </c>
       <c r="G166" s="37" t="s">
         <v>443</v>
@@ -17300,27 +17300,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17578,10 +17557,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17604,20 +17615,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fix campi test case 24
</commit_message>
<xml_diff>
--- a/GATEWAY/SIG120200_00987654321-AppTest01/Replycare s.r.l./Med58/V.1.0.0/report-checklist.xlsx
+++ b/GATEWAY/SIG120200_00987654321-AppTest01/Replycare s.r.l./Med58/V.1.0.0/report-checklist.xlsx
@@ -1730,13 +1730,13 @@
     <t>Errore durante il caricamento del documento. C'è stato un errore durante la comunicazione con il Fascicolo Sanitario Elettronico, la preghiamo di [riprovare la procedura. Se l'errore persiste] comunicare con support@med58.com</t>
   </si>
   <si>
-    <t>2025-09-26T08:21:21Z</t>
-  </si>
-  <si>
-    <t>0c954291f541b83ca696ca51fa658e2c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.29ccee2c841f0f1da2c46f6c1109bfa24bb68da0edf9f5e7a0b17dfae32dde40.85bf595908^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-09-26T15:11:53Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.f08192632027d5956ed6a07d68b06d48f6dae1379c77abcb01ca7abb3201bccf.391d74591f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>914cd92fb3b35d1740d72a15d0e407d1</t>
   </si>
 </sst>
 </file>
@@ -3806,10 +3806,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I166" sqref="I166"/>
+      <selection pane="bottomRight" activeCell="I167" sqref="I167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9991,10 +9991,10 @@
         <v>443</v>
       </c>
       <c r="H166" s="37" t="s">
+        <v>445</v>
+      </c>
+      <c r="I166" s="42" t="s">
         <v>444</v>
-      </c>
-      <c r="I166" s="42" t="s">
-        <v>445</v>
       </c>
       <c r="J166" s="38" t="s">
         <v>64</v>

</xml_diff>